<commit_message>
literature search and behavior paradigm
</commit_message>
<xml_diff>
--- a/LiteratureSearch/LiteratureSearch.xlsx
+++ b/LiteratureSearch/LiteratureSearch.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="22995" windowHeight="12585"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20730" windowHeight="11745"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="papers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="58">
   <si>
     <t>Paper</t>
   </si>
@@ -25,9 +25,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t>gene expression &amp; leanring</t>
-  </si>
-  <si>
     <t>CA1</t>
   </si>
   <si>
@@ -47,17 +44,174 @@
   </si>
   <si>
     <t>calcium signalling CA1 pyramidal</t>
+  </si>
+  <si>
+    <t>gene expression &amp; learning</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Denny et al 2014</t>
+  </si>
+  <si>
+    <t>memory traces are located in the DG and in CA3 but that the strength of the memory is related to reactivation in CA3</t>
+  </si>
+  <si>
+    <t>Lein et al 2007</t>
+  </si>
+  <si>
+    <t>wfs1</t>
+  </si>
+  <si>
+    <t>map3k15</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>behavior??</t>
+  </si>
+  <si>
+    <t>collect tissue?</t>
+  </si>
+  <si>
+    <t>animal</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>human</t>
+  </si>
+  <si>
+    <t>laser microdissection</t>
+  </si>
+  <si>
+    <t>donors</t>
+  </si>
+  <si>
+    <t>gene expresssion</t>
+  </si>
+  <si>
+    <t>microarray</t>
+  </si>
+  <si>
+    <t>C57BL/6J mice</t>
+  </si>
+  <si>
+    <t>homecage</t>
+  </si>
+  <si>
+    <t>Hawrylycz et al. 2012</t>
+  </si>
+  <si>
+    <t>CALB1</t>
+  </si>
+  <si>
+    <t>adult mouse</t>
+  </si>
+  <si>
+    <t>rhesus macaque</t>
+  </si>
+  <si>
+    <t>ISH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA3 and CA4 subfields were not discriminable </t>
+  </si>
+  <si>
+    <t>discrete subdivisions show distinctive expressions sufficiently robust to cluster together like-samples while distinguishing subdivisions from one another</t>
+  </si>
+  <si>
+    <t>fresh-frozen cryostat sections</t>
+  </si>
+  <si>
+    <t>Pvrl3</t>
+  </si>
+  <si>
+    <t>Col15a1 (expressed in a gradient with higher expression proximal to DG)</t>
+  </si>
+  <si>
+    <t>Crym (expressed in a reciprocal gradient to Col15a1)</t>
+  </si>
+  <si>
+    <t>Col6a1 (selective expression in the outer band of cells in CA2(?) and CA3</t>
+  </si>
+  <si>
+    <t>x (?)</t>
+  </si>
+  <si>
+    <t>Dorsal</t>
+  </si>
+  <si>
+    <t>Ventral</t>
+  </si>
+  <si>
+    <t>Dsp (neuropeptide) (differential expression in granule cells)</t>
+  </si>
+  <si>
+    <t>Grp (neuropeptide) (differential expression in granule cells)</t>
+  </si>
+  <si>
+    <t>Nmb (differential expression in hilar neurons)</t>
+  </si>
+  <si>
+    <t>Slit2 (differential expression in hilar neurons)</t>
+  </si>
+  <si>
+    <t>*5 out of 10 genes shown in this figure involved in cell adhesion*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mRNA targeting </t>
+  </si>
+  <si>
+    <t>Nptx1 (confined to soma of CA3 pyramidal cells)</t>
+  </si>
+  <si>
+    <t>Mtap1a (proximal apical dendrite)</t>
+  </si>
+  <si>
+    <t>Mtap2 (proximal and distal dendrites)</t>
+  </si>
+  <si>
+    <t>http://www.nature.com/nature/journal/v445/n7124/fig_tab/nature05453_F9.html</t>
+  </si>
+  <si>
+    <t>http://www.nature.com/nature/journal/v445/n7124/fig_tab/nature05453_F7.html</t>
+  </si>
+  <si>
+    <t>http://www.nature.com/nature/journal/v489/n7416/fig_tab/nature11405_F5.html</t>
+  </si>
+  <si>
+    <t>Camk2a (apical and basal dendritic zones)</t>
+  </si>
+  <si>
+    <t>Dnd1 (apical and basal dendritic zones)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -78,13 +232,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,19 +549,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B9:B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,38 +569,641 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" t="s">
+        <v>33</v>
+      </c>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" t="s">
+        <v>49</v>
+      </c>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
+        <v>32</v>
+      </c>
+      <c r="L22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M10" r:id="rId1"/>
+    <hyperlink ref="M23" r:id="rId2"/>
+    <hyperlink ref="M15" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>